<commit_message>
Changed excel file to match new schema
</commit_message>
<xml_diff>
--- a/Presentation.Web/Content/excel/OS2KITOS IT Kontrakter.xlsx
+++ b/Presentation.Web/Content/excel/OS2KITOS IT Kontrakter.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESD\Source\Repos\kitos\Presentation.Web\Content\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\source\KITOS\Presentation.Web\Content\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B599926-17FD-402C-A8E5-748F50F3E55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24750" windowHeight="12330"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT Kontrakter" sheetId="1" r:id="rId1"/>
@@ -24,15 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>IT Kontrakt Id</t>
-  </si>
-  <si>
-    <t>ESDH ref.</t>
-  </si>
-  <si>
-    <t>Mappe</t>
   </si>
   <si>
     <t>Bemærkning</t>
@@ -73,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -145,8 +140,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Overskrift 1" xfId="1" builtinId="16"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -423,35 +418,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -459,10 +454,10 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -471,18 +466,12 @@
       <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0"/>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:J1048576">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J1048576 E1:H1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>29221</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>